<commit_message>
Added Functionality to TS GA
Need to implement some type of ordered system...python dictionaries are
not ordered.
</commit_message>
<xml_diff>
--- a/Traveling Salesman.xlsx
+++ b/Traveling Salesman.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\souleke\Desktop\GitHub\Capacity-Planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\namestaken\Documents\GitHub\Capacity-Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>x</t>
   </si>
@@ -33,6 +33,117 @@
   </si>
   <si>
     <t>Point</t>
+  </si>
+  <si>
+    <t>C10(100,160)</t>
+  </si>
+  <si>
+    <t>C17(100,40)</t>
+  </si>
+  <si>
+    <t>C18(200,160)</t>
+  </si>
+  <si>
+    <t>C11(120,80)</t>
+  </si>
+  <si>
+    <t>C19(200,40)</t>
+  </si>
+  <si>
+    <t>C16(180,100)</t>
+  </si>
+  <si>
+    <t>C13(180,60)</t>
+  </si>
+  <si>
+    <t>C9(20,160)</t>
+  </si>
+  <si>
+    <t>C8(140,140)</t>
+  </si>
+  <si>
+    <t>C14(180,200)</t>
+  </si>
+  <si>
+    <t>C15(160,20)</t>
+  </si>
+  <si>
+    <t>C12(140,180)</t>
+  </si>
+  <si>
+    <t>C3(40,120)</t>
+  </si>
+  <si>
+    <t>C2(20,40)</t>
+  </si>
+  <si>
+    <t>C1(60,20)</t>
+  </si>
+  <si>
+    <t>C0(20,20)</t>
+  </si>
+  <si>
+    <t>C7(80,180)</t>
+  </si>
+  <si>
+    <t>C6(100,120)</t>
+  </si>
+  <si>
+    <t>C5(60,200)</t>
+  </si>
+  <si>
+    <t>C4(60,80)</t>
+  </si>
+  <si>
+    <t>C17(200,160)</t>
+  </si>
+  <si>
+    <t>C18(120,80)</t>
+  </si>
+  <si>
+    <t>C11(200,40)</t>
+  </si>
+  <si>
+    <t>C19(180,100)</t>
+  </si>
+  <si>
+    <t>C16(180,60)</t>
+  </si>
+  <si>
+    <t>C13(100,40)</t>
+  </si>
+  <si>
+    <t>C9(140,140)</t>
+  </si>
+  <si>
+    <t>C8(180,200)</t>
+  </si>
+  <si>
+    <t>C14(20,160)</t>
+  </si>
+  <si>
+    <t>C3(20,40)</t>
+  </si>
+  <si>
+    <t>C2(40,120)</t>
+  </si>
+  <si>
+    <t>C1(20,20)</t>
+  </si>
+  <si>
+    <t>C0(80,180)</t>
+  </si>
+  <si>
+    <t>C7(100,120)</t>
+  </si>
+  <si>
+    <t>C6(60,20)</t>
+  </si>
+  <si>
+    <t>C5(60,80)</t>
+  </si>
+  <si>
+    <t>C4(60,200)</t>
   </si>
 </sst>
 </file>
@@ -455,9 +566,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -465,7 +578,7 @@
     <col min="2" max="3" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -475,8 +588,21 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="b">
+        <f>AND(O1 = Q1, Q1 = S1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -486,8 +612,21 @@
       <c r="C2">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" t="b">
+        <f t="shared" ref="U2:U20" si="0">AND(O2 = Q2, Q2 = S2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -497,8 +636,21 @@
       <c r="C3">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>2</v>
@@ -509,10 +661,23 @@
       <c r="C4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A21" si="0">A4+1</f>
+        <f t="shared" ref="A5:A21" si="1">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="4">
@@ -521,10 +686,23 @@
       <c r="C5">
         <v>120</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>7</v>
+      </c>
+      <c r="S5" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" s="4">
@@ -533,10 +711,23 @@
       <c r="C6">
         <v>200</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" t="s">
+        <v>27</v>
+      </c>
+      <c r="U6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7" s="4">
@@ -545,10 +736,23 @@
       <c r="C7">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>9</v>
+      </c>
+      <c r="S7" t="s">
+        <v>28</v>
+      </c>
+      <c r="U7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8" s="4">
@@ -557,10 +761,23 @@
       <c r="C8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S8" t="s">
+        <v>29</v>
+      </c>
+      <c r="U8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9" s="4">
@@ -569,10 +786,23 @@
       <c r="C9">
         <v>180</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>11</v>
+      </c>
+      <c r="S9" t="s">
+        <v>30</v>
+      </c>
+      <c r="U9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10" s="4">
@@ -581,10 +811,23 @@
       <c r="C10">
         <v>160</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" t="s">
+        <v>31</v>
+      </c>
+      <c r="U10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11" s="4">
@@ -593,10 +836,23 @@
       <c r="C11">
         <v>120</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S11" t="s">
+        <v>13</v>
+      </c>
+      <c r="U11" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="4">
@@ -605,10 +861,23 @@
       <c r="C12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O12" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>14</v>
+      </c>
+      <c r="S12" t="s">
+        <v>14</v>
+      </c>
+      <c r="U12" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13" s="4">
@@ -617,10 +886,23 @@
       <c r="C13">
         <v>80</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" t="s">
+        <v>32</v>
+      </c>
+      <c r="U13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14" s="4">
@@ -629,10 +911,23 @@
       <c r="C14">
         <v>180</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>16</v>
+      </c>
+      <c r="S14" t="s">
+        <v>33</v>
+      </c>
+      <c r="U14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15" s="4">
@@ -641,10 +936,23 @@
       <c r="C15">
         <v>140</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" t="s">
+        <v>34</v>
+      </c>
+      <c r="U15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16" s="4">
@@ -653,10 +961,23 @@
       <c r="C16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16" t="s">
+        <v>35</v>
+      </c>
+      <c r="U16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17" s="4">
@@ -665,10 +986,23 @@
       <c r="C17">
         <v>200</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
+        <v>36</v>
+      </c>
+      <c r="U17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18" s="4">
@@ -677,10 +1011,23 @@
       <c r="C18">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>20</v>
+      </c>
+      <c r="S18" t="s">
+        <v>37</v>
+      </c>
+      <c r="U18" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19" s="4">
@@ -689,10 +1036,23 @@
       <c r="C19">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>21</v>
+      </c>
+      <c r="S19" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20" s="4">
@@ -701,10 +1061,23 @@
       <c r="C20">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="O20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>22</v>
+      </c>
+      <c r="S20" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21" s="4">

</xml_diff>